<commit_message>
Continuing to add upgrade code
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Fusion Cooling</t>
   </si>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,15 +528,24 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>